<commit_message>
añadimos estilos css a los botones de las nominas persistentes
</commit_message>
<xml_diff>
--- a/nominas_persistentes.xlsx
+++ b/nominas_persistentes.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,510 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>11027335</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ORBACH ALBERTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>HUGO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>33920521</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OSORIO MARTIN</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HORACIO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>28029403</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OZUNA WALTER</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OSCAR</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>04703477</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PASETTO FERNANDO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>LAZARO</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>16354298</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PEREA ROGELIO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ELADIO</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12600144</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>POLAKIEWICK SERGIO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MARIO</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28454779</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ROJAS JUAN</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>OSCAR</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>28592127</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ROMERO DIEGO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>RAUL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>31738492</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ROMERO JUAN</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CARLOS</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>45623997</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SANTILLAN DIEGO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ANTONIO</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>94720639</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SILVERO MARIO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>RAMON</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>38691218</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SORIA FABIO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>OSVALDO</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>20550320</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SOSA CARLOS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>JESUS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>41880461</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SOSA KEVIN</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ALEJANDRO</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>94439309</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TICONA CALDERON</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>DANIEL</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>18579333</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>UEHARA MARIA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CRISTINA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>39588571</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>VALENCIA FRANCO</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>EZEQUIEL</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>41988092</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>VALENCIA LAUTARO</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NAHUEL</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Mecan Se</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>46336</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>46023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>